<commit_message>
:tada: feat: add music effect
</commit_message>
<xml_diff>
--- a/users.xlsx
+++ b/users.xlsx
@@ -4,14 +4,27 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="15860"/>
+    <workbookView windowHeight="17655"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -1591,11 +1604,11 @@
       <selection activeCell="E68" sqref="E68"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="2"/>
   <cols>
-    <col min="1" max="1" width="58.9711538461538" customWidth="1"/>
-    <col min="2" max="2" width="28.3653846153846" customWidth="1"/>
-    <col min="3" max="3" width="27.8846153846154" customWidth="1"/>
+    <col min="1" max="1" width="25.125" customWidth="1"/>
+    <col min="2" max="2" width="17.375" customWidth="1"/>
+    <col min="3" max="3" width="27.8833333333333" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -2395,7 +2408,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
@@ -2412,7 +2425,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>